<commit_message>
Updated Content Management - Social
</commit_message>
<xml_diff>
--- a/data/Social_Engagement.xlsx
+++ b/data/Social_Engagement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{291B5E37-035A-4DFC-8CDA-3926D1990E74}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{73A2D24A-73DF-4DCC-A4DD-7E2BA228DC01}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
     <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>Unpublished Type</t>
   </si>
@@ -48,10 +48,28 @@
     <t>Posts</t>
   </si>
   <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Replies</t>
+  </si>
+  <si>
+    <t>Rohit Menon</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Rejected</t>
+  </si>
+  <si>
+    <t>Post Error</t>
+  </si>
+  <si>
     <t>Pending Approval</t>
   </si>
   <si>
-    <t>Sanjeev Kanna</t>
+    <t>Approved Scheduled</t>
   </si>
 </sst>
 </file>
@@ -379,17 +397,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
   </cols>
@@ -413,19 +431,70 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>6</v>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Filter file and Social Test Data
</commit_message>
<xml_diff>
--- a/data/Social_Engagement.xlsx
+++ b/data/Social_Engagement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{73A2D24A-73DF-4DCC-A4DD-7E2BA228DC01}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{49C1E283-C2AA-4B17-9269-F950A2BBFA8D}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
     <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Unpublished Type</t>
   </si>
@@ -51,25 +51,10 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Replies</t>
-  </si>
-  <si>
     <t>Rohit Menon</t>
   </si>
   <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>Rejected</t>
-  </si>
-  <si>
-    <t>Post Error</t>
-  </si>
-  <si>
     <t>Pending Approval</t>
-  </si>
-  <si>
-    <t>Approved Scheduled</t>
   </si>
 </sst>
 </file>
@@ -397,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="A3" sqref="A3:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,70 +416,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created and Updated Reviews Feed: Respond to Reviews Scenarios
</commit_message>
<xml_diff>
--- a/data/Social_Engagement.xlsx
+++ b/data/Social_Engagement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avinash\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{49C1E283-C2AA-4B17-9269-F950A2BBFA8D}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{CD242623-2050-41A8-B277-67FFFCED5C38}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46"/>
   <bookViews>
     <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Unpublished Type</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Comments</t>
-  </si>
-  <si>
-    <t>Rohit Menon</t>
   </si>
   <si>
     <t>Pending Approval</t>
@@ -385,7 +382,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,13 +413,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>

</xml_diff>